<commit_message>
Translated the xslx file
</commit_message>
<xml_diff>
--- a/files/history.xlsx
+++ b/files/history.xlsx
@@ -26,37 +26,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Kauba nimi</t>
-  </si>
-  <si>
-    <t>Aeg</t>
-  </si>
-  <si>
-    <t>Koht</t>
-  </si>
-  <si>
-    <t>Piim</t>
-  </si>
-  <si>
-    <t>Kesklinna kauplus</t>
-  </si>
-  <si>
-    <t>Sai</t>
-  </si>
-  <si>
-    <t>Ülemiste kauplus</t>
-  </si>
-  <si>
-    <t>Leib</t>
-  </si>
-  <si>
-    <t>Lasnamäe kauplus</t>
-  </si>
-  <si>
-    <t>Õlu</t>
-  </si>
-  <si>
-    <t>Nõmme pood</t>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>White bread</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Nõmme store</t>
+  </si>
+  <si>
+    <t>Kesklinna store</t>
+  </si>
+  <si>
+    <t>Ülemiste store</t>
+  </si>
+  <si>
+    <t>Lasnamäe store</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,16 +419,16 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -436,7 +436,7 @@
         <v>42736.538194444445</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,29 +447,29 @@
         <v>42736.538194444445</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>42736.538194444445</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>42736.538194444445</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>